<commit_message>
feat [faculty][dashboard]: chart 4 top students
</commit_message>
<xml_diff>
--- a/DATA/faculty-data-format.xlsx
+++ b/DATA/faculty-data-format.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\Grading-Management-System\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Grading-Management-System\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8510" windowHeight="5760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8505" windowHeight="5760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="21">
   <si>
     <t>Employee ID</t>
   </si>
@@ -44,73 +44,49 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>rico@gmail.com</t>
-  </si>
-  <si>
     <t>09239297567</t>
   </si>
   <si>
-    <t>09256866233</t>
-  </si>
-  <si>
-    <t>loida@gmail.com</t>
-  </si>
-  <si>
-    <t>09258966257</t>
-  </si>
-  <si>
-    <t>rowena@gmail.com</t>
-  </si>
-  <si>
-    <t>nico@gmail.com</t>
-  </si>
-  <si>
-    <t>09675436789</t>
-  </si>
-  <si>
-    <t>09765456782</t>
-  </si>
-  <si>
     <t>IT 401</t>
   </si>
   <si>
     <t>IT 402</t>
   </si>
   <si>
-    <t>IT 403</t>
-  </si>
-  <si>
-    <t>IT 404</t>
-  </si>
-  <si>
-    <t>IT 405</t>
-  </si>
-  <si>
-    <t>4A, 4E, 4F</t>
-  </si>
-  <si>
-    <t>4A, 4B, 4C, 4D</t>
-  </si>
-  <si>
-    <t>4A, 4C, 4F, 4G</t>
-  </si>
-  <si>
     <t>Esguerra, Lucy</t>
   </si>
   <si>
-    <t>Cruz, Rico</t>
-  </si>
-  <si>
-    <t>Santos, Loisa</t>
-  </si>
-  <si>
-    <t>Reyes, Rowena</t>
-  </si>
-  <si>
-    <t>Dela Cruz, Nico</t>
-  </si>
-  <si>
     <t>lucyesguerra972@gmail.com</t>
+  </si>
+  <si>
+    <t>1A, 1B, 1C</t>
+  </si>
+  <si>
+    <t>NSTP 10</t>
+  </si>
+  <si>
+    <t>IT 102</t>
+  </si>
+  <si>
+    <t>IT 103</t>
+  </si>
+  <si>
+    <t>IT 104</t>
+  </si>
+  <si>
+    <t>RPH 101</t>
+  </si>
+  <si>
+    <t>AAP 101</t>
+  </si>
+  <si>
+    <t>STS 101</t>
+  </si>
+  <si>
+    <t>ARP 101</t>
+  </si>
+  <si>
+    <t>PE 10</t>
   </si>
 </sst>
 </file>
@@ -492,24 +468,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="3" customWidth="1"/>
     <col min="3" max="3" width="17" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="4" max="4" width="14.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -529,156 +505,237 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>2018919156</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7">
-        <v>2018919156</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7">
-        <v>2018234567</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7">
-        <v>2018667545</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="7">
-        <v>2018667096</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
-        <v>2018667546</v>
+        <v>2018919156</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4"/>
-    <hyperlink ref="C7" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C8" r:id="rId4"/>
+    <hyperlink ref="C10" r:id="rId5"/>
+    <hyperlink ref="C12" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
style [admin][dashboard]: Charts and tables
</commit_message>
<xml_diff>
--- a/DATA/faculty-data-format.xlsx
+++ b/DATA/faculty-data-format.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="66">
   <si>
     <t>Employee ID</t>
   </si>
@@ -87,6 +87,141 @@
   </si>
   <si>
     <t>PE 10</t>
+  </si>
+  <si>
+    <t>IT 403</t>
+  </si>
+  <si>
+    <t>CAP 401</t>
+  </si>
+  <si>
+    <t>IT 404</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>IT 301</t>
+  </si>
+  <si>
+    <t>IT 302</t>
+  </si>
+  <si>
+    <t>IT 303</t>
+  </si>
+  <si>
+    <t>IT 304</t>
+  </si>
+  <si>
+    <t>IT 305</t>
+  </si>
+  <si>
+    <t>IT 306</t>
+  </si>
+  <si>
+    <t>IT 307</t>
+  </si>
+  <si>
+    <t>FL 301</t>
+  </si>
+  <si>
+    <t>IT 308</t>
+  </si>
+  <si>
+    <t>IT 309</t>
+  </si>
+  <si>
+    <t>IT 310</t>
+  </si>
+  <si>
+    <t>CAP 301</t>
+  </si>
+  <si>
+    <t>IT 311</t>
+  </si>
+  <si>
+    <t>IT312</t>
+  </si>
+  <si>
+    <t>FL 302</t>
+  </si>
+  <si>
+    <t>RLW 101</t>
+  </si>
+  <si>
+    <t>IT 105</t>
+  </si>
+  <si>
+    <t>IT 106</t>
+  </si>
+  <si>
+    <t>IT 107</t>
+  </si>
+  <si>
+    <t>PCM 101</t>
+  </si>
+  <si>
+    <t>MMW 101</t>
+  </si>
+  <si>
+    <t>UTS 101</t>
+  </si>
+  <si>
+    <t>PAL101</t>
+  </si>
+  <si>
+    <t>PE 11</t>
+  </si>
+  <si>
+    <t>NSTP 11</t>
+  </si>
+  <si>
+    <t>IT 201</t>
+  </si>
+  <si>
+    <t>IT 202</t>
+  </si>
+  <si>
+    <t>IT 203</t>
+  </si>
+  <si>
+    <t>IT 204</t>
+  </si>
+  <si>
+    <t>IT205</t>
+  </si>
+  <si>
+    <t>AAH 101d*</t>
+  </si>
+  <si>
+    <t>ETH 101</t>
+  </si>
+  <si>
+    <t>PE 12</t>
+  </si>
+  <si>
+    <t>IT 206</t>
+  </si>
+  <si>
+    <t>IT 207</t>
+  </si>
+  <si>
+    <t>IT 208</t>
+  </si>
+  <si>
+    <t>IT 209</t>
+  </si>
+  <si>
+    <t>IT 210</t>
+  </si>
+  <si>
+    <t>TCW 101</t>
+  </si>
+  <si>
+    <t>MST 101d*</t>
+  </si>
+  <si>
+    <t>PE 13</t>
   </si>
 </sst>
 </file>
@@ -468,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A10" sqref="A10:A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,6 +860,1106 @@
         <v>11</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>63</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>28</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" t="s">
+        <v>30</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" t="s">
+        <v>31</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" t="s">
+        <v>32</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" t="s">
+        <v>33</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" t="s">
+        <v>34</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" t="s">
+        <v>36</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" t="s">
+        <v>37</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" t="s">
+        <v>38</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" t="s">
+        <v>39</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
+        <v>21</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
+        <v>2018919156</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>23</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -734,8 +1969,63 @@
     <hyperlink ref="C8" r:id="rId4"/>
     <hyperlink ref="C10" r:id="rId5"/>
     <hyperlink ref="C12" r:id="rId6"/>
+    <hyperlink ref="C13" r:id="rId7"/>
+    <hyperlink ref="C14" r:id="rId8"/>
+    <hyperlink ref="C15" r:id="rId9"/>
+    <hyperlink ref="C16" r:id="rId10"/>
+    <hyperlink ref="C17" r:id="rId11"/>
+    <hyperlink ref="C18" r:id="rId12"/>
+    <hyperlink ref="C19" r:id="rId13"/>
+    <hyperlink ref="C20" r:id="rId14"/>
+    <hyperlink ref="C21" r:id="rId15"/>
+    <hyperlink ref="C22" r:id="rId16"/>
+    <hyperlink ref="C23" r:id="rId17"/>
+    <hyperlink ref="C24" r:id="rId18"/>
+    <hyperlink ref="C25" r:id="rId19"/>
+    <hyperlink ref="C26" r:id="rId20"/>
+    <hyperlink ref="C27" r:id="rId21"/>
+    <hyperlink ref="C28" r:id="rId22"/>
+    <hyperlink ref="C29" r:id="rId23"/>
+    <hyperlink ref="C30" r:id="rId24"/>
+    <hyperlink ref="C31" r:id="rId25"/>
+    <hyperlink ref="C32" r:id="rId26"/>
+    <hyperlink ref="C33" r:id="rId27"/>
+    <hyperlink ref="C34" r:id="rId28"/>
+    <hyperlink ref="C35" r:id="rId29"/>
+    <hyperlink ref="C36" r:id="rId30"/>
+    <hyperlink ref="C37" r:id="rId31"/>
+    <hyperlink ref="C38" r:id="rId32"/>
+    <hyperlink ref="C39" r:id="rId33"/>
+    <hyperlink ref="C40" r:id="rId34"/>
+    <hyperlink ref="C41" r:id="rId35"/>
+    <hyperlink ref="C42" r:id="rId36"/>
+    <hyperlink ref="C43" r:id="rId37"/>
+    <hyperlink ref="C44" r:id="rId38"/>
+    <hyperlink ref="C45" r:id="rId39"/>
+    <hyperlink ref="C46" r:id="rId40"/>
+    <hyperlink ref="C47" r:id="rId41"/>
+    <hyperlink ref="C48" r:id="rId42"/>
+    <hyperlink ref="C49" r:id="rId43"/>
+    <hyperlink ref="C50" r:id="rId44"/>
+    <hyperlink ref="C51" r:id="rId45"/>
+    <hyperlink ref="C52" r:id="rId46"/>
+    <hyperlink ref="C53" r:id="rId47"/>
+    <hyperlink ref="C54" r:id="rId48"/>
+    <hyperlink ref="C55" r:id="rId49"/>
+    <hyperlink ref="C56" r:id="rId50"/>
+    <hyperlink ref="C57" r:id="rId51"/>
+    <hyperlink ref="C58" r:id="rId52"/>
+    <hyperlink ref="C59" r:id="rId53"/>
+    <hyperlink ref="C60" r:id="rId54"/>
+    <hyperlink ref="C61" r:id="rId55"/>
+    <hyperlink ref="C62" r:id="rId56"/>
+    <hyperlink ref="C63" r:id="rId57"/>
+    <hyperlink ref="C64" r:id="rId58"/>
+    <hyperlink ref="C65" r:id="rId59"/>
+    <hyperlink ref="C66" r:id="rId60"/>
+    <hyperlink ref="C67" r:id="rId61"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId62"/>
 </worksheet>
 </file>
</xml_diff>